<commit_message>
updated railway-freight and inlandshipping data
</commit_message>
<xml_diff>
--- a/data/mobility/raw_data/Eisenbahngüterverkehr_monatlich.xlsx
+++ b/data/mobility/raw_data/Eisenbahngüterverkehr_monatlich.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph\Desktop\3. Semester\Applied Machine Intelligence\Semester Project\Data_preprocessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph\Desktop\3. Semester\Applied Machine Intelligence\Semester Project\Data_preprocessing\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8849158A-01C7-4975-926D-BBFD06CF094C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA6028E5-2544-4E15-85E3-2CA668E5CD19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392"/>
   </bookViews>
   <sheets>
-    <sheet name="Eisenbahngüterverkehr_monatlich" sheetId="1" r:id="rId1"/>
+    <sheet name="46131-0004" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="31">
   <si>
     <t>GENESIS-Tabelle: 46131-0004</t>
   </si>
@@ -112,7 +112,7 @@
     <t>© Statistisches Bundesamt (Destatis), 2020</t>
   </si>
   <si>
-    <t>Stand: 19.06.2020 / 12:18:53</t>
+    <t>Stand: 06.07.2020 / 16:14:31</t>
   </si>
 </sst>
 </file>
@@ -8040,35 +8040,35 @@
       <c r="B193" t="s">
         <v>17</v>
       </c>
-      <c r="C193" t="s">
-        <v>27</v>
-      </c>
-      <c r="D193" t="s">
-        <v>27</v>
-      </c>
-      <c r="E193" t="s">
-        <v>27</v>
-      </c>
-      <c r="F193" t="s">
-        <v>27</v>
-      </c>
-      <c r="G193" t="s">
-        <v>27</v>
-      </c>
-      <c r="H193" t="s">
-        <v>27</v>
-      </c>
-      <c r="I193" t="s">
-        <v>27</v>
-      </c>
-      <c r="J193" t="s">
-        <v>27</v>
-      </c>
-      <c r="K193" t="s">
-        <v>27</v>
-      </c>
-      <c r="L193" t="s">
-        <v>27</v>
+      <c r="C193">
+        <v>19137355</v>
+      </c>
+      <c r="D193">
+        <v>4941670397</v>
+      </c>
+      <c r="E193">
+        <v>3955618</v>
+      </c>
+      <c r="F193">
+        <v>1916175746</v>
+      </c>
+      <c r="G193">
+        <v>4775905</v>
+      </c>
+      <c r="H193">
+        <v>2071593829</v>
+      </c>
+      <c r="I193">
+        <v>1896470</v>
+      </c>
+      <c r="J193">
+        <v>1192333457</v>
+      </c>
+      <c r="K193">
+        <v>29765348</v>
+      </c>
+      <c r="L193">
+        <v>10121773429</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.55000000000000004">

</xml_diff>